<commit_message>
filtro de consumidor corregido
</commit_message>
<xml_diff>
--- a/desarrollo/rigk-sg-back/files/templates/Declaraciones_CI_YYYY.xlsx
+++ b/desarrollo/rigk-sg-back/files/templates/Declaraciones_CI_YYYY.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2430" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2556" uniqueCount="397">
   <si>
     <t>ID empresa</t>
   </si>
@@ -598,6 +598,18 @@
     <t>77934420-7</t>
   </si>
   <si>
+    <t>ZZ3</t>
+  </si>
+  <si>
+    <t>EMPRESA ZZ3</t>
+  </si>
+  <si>
+    <t>est zz3</t>
+  </si>
+  <si>
+    <t>ZORO Z2 ZORTO</t>
+  </si>
+  <si>
     <t>PR-2</t>
   </si>
   <si>
@@ -1030,6 +1042,12 @@
     <t>empresa dashboard 2</t>
   </si>
   <si>
+    <t>tm-2</t>
+  </si>
+  <si>
+    <t>tomas2</t>
+  </si>
+  <si>
     <t>Notas: Todo en Toneladas. Totales anuales del año de ejercicio (año que se declara)</t>
   </si>
   <si>
@@ -1045,19 +1063,19 @@
     <t>Peso Total Declarado</t>
   </si>
   <si>
-    <t>11158413,70</t>
+    <t>11164413,70</t>
   </si>
   <si>
     <t>Peso Total Valorizado</t>
   </si>
   <si>
-    <t>1048254,43</t>
+    <t>1049254,43</t>
   </si>
   <si>
     <t xml:space="preserve">Total Reciclaje Papel/Cartón (Reciclaje Mecánico + Reciclaje Interno) </t>
   </si>
   <si>
-    <t>1017000,11</t>
+    <t>1019000,11</t>
   </si>
   <si>
     <t xml:space="preserve">Total Reciclaje Plástico (Reciclaje Mecánico + Reciclaje Interno) </t>
@@ -1108,7 +1126,7 @@
     <t>Total no valorizado Papel/Cartón (Disposicion Final en RS +  DF en Relleno Seguridad)</t>
   </si>
   <si>
-    <t>29000,00</t>
+    <t>31000,00</t>
   </si>
   <si>
     <t>Total no valorizado Plastico (Disposicion Final en RS + DF en Relleno Seguridad)</t>
@@ -1135,7 +1153,7 @@
     <t>Total preparación para reutilización por todas las subcategoría (Disposicion Final en RS + DF en Relleno Seguridad)</t>
   </si>
   <si>
-    <t>5065200,44</t>
+    <t>5067200,44</t>
   </si>
   <si>
     <t xml:space="preserve">Total Valorización Región de Arica y Parinacota  (Reciclaje Mecánico + Reciclaje Interno + Valorizacion Energetica) </t>
@@ -1566,7 +1584,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R131"/>
+  <dimension ref="A1:R138"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
@@ -2505,7 +2523,7 @@
         <v>25</v>
       </c>
       <c r="I17" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="J17" t="s">
         <v>27</v>
@@ -2520,7 +2538,7 @@
         <v>83</v>
       </c>
       <c r="N17" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="O17" t="s">
         <v>84</v>
@@ -4948,346 +4966,346 @@
         <v>194</v>
       </c>
       <c r="B61" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" t="s">
         <v>195</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>196</v>
       </c>
-      <c r="D61" t="s">
-        <v>31</v>
-      </c>
       <c r="E61" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F61" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G61" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="H61" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="I61" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J61" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K61" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L61" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M61" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="N61" t="s">
         <v>31</v>
       </c>
       <c r="O61" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="P61" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Q61" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="R61" t="s">
-        <v>31</v>
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>194</v>
+      </c>
+      <c r="B62" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" t="s">
+        <v>195</v>
+      </c>
+      <c r="D62" t="s">
+        <v>196</v>
+      </c>
+      <c r="E62" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" t="s">
+        <v>23</v>
+      </c>
+      <c r="G62" t="s">
+        <v>132</v>
+      </c>
+      <c r="H62" t="s">
+        <v>25</v>
+      </c>
+      <c r="I62" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" t="s">
+        <v>27</v>
+      </c>
+      <c r="K62" t="s">
+        <v>40</v>
+      </c>
+      <c r="L62" t="s">
+        <v>85</v>
+      </c>
+      <c r="M62" t="s">
+        <v>83</v>
+      </c>
+      <c r="N62" t="s">
+        <v>31</v>
+      </c>
+      <c r="O62" t="s">
+        <v>113</v>
+      </c>
+      <c r="P62" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>87</v>
+      </c>
+      <c r="R62" t="s">
         <v>197</v>
-      </c>
-      <c r="B62" t="s">
-        <v>48</v>
-      </c>
-      <c r="C62" t="s">
-        <v>198</v>
-      </c>
-      <c r="D62" t="s">
-        <v>31</v>
-      </c>
-      <c r="E62" t="s">
-        <v>31</v>
-      </c>
-      <c r="F62" t="s">
-        <v>31</v>
-      </c>
-      <c r="G62" t="s">
-        <v>31</v>
-      </c>
-      <c r="H62" t="s">
-        <v>31</v>
-      </c>
-      <c r="I62" t="s">
-        <v>31</v>
-      </c>
-      <c r="J62" t="s">
-        <v>31</v>
-      </c>
-      <c r="K62" t="s">
-        <v>31</v>
-      </c>
-      <c r="L62" t="s">
-        <v>31</v>
-      </c>
-      <c r="M62" t="s">
-        <v>31</v>
-      </c>
-      <c r="N62" t="s">
-        <v>31</v>
-      </c>
-      <c r="O62" t="s">
-        <v>31</v>
-      </c>
-      <c r="P62" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>31</v>
-      </c>
-      <c r="R62" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B63" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C63" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D63" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="E63" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F63" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G63" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="H63" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="I63" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J63" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K63" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="L63" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="M63" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="N63" t="s">
         <v>31</v>
       </c>
       <c r="O63" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="P63" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="Q63" t="s">
-        <v>31</v>
+        <v>90</v>
       </c>
       <c r="R63" t="s">
-        <v>31</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="B64" t="s">
         <v>19</v>
       </c>
       <c r="C64" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="D64" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="E64" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F64" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G64" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="H64" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="I64" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J64" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K64" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="L64" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="M64" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="N64" t="s">
         <v>31</v>
       </c>
       <c r="O64" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="P64" t="s">
-        <v>31</v>
+        <v>93</v>
       </c>
       <c r="Q64" t="s">
-        <v>31</v>
+        <v>94</v>
       </c>
       <c r="R64" t="s">
-        <v>31</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B65" t="s">
         <v>19</v>
       </c>
       <c r="C65" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D65" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="E65" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F65" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G65" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="H65" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="I65" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J65" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K65" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="L65" t="s">
-        <v>31</v>
+        <v>96</v>
       </c>
       <c r="M65" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="N65" t="s">
         <v>31</v>
       </c>
       <c r="O65" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="P65" t="s">
-        <v>31</v>
+        <v>97</v>
       </c>
       <c r="Q65" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="R65" t="s">
-        <v>31</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B66" t="s">
         <v>19</v>
       </c>
       <c r="C66" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="D66" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="E66" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F66" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G66" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="H66" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="I66" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J66" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K66" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="L66" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="M66" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="N66" t="s">
         <v>31</v>
       </c>
       <c r="O66" t="s">
-        <v>31</v>
+        <v>113</v>
       </c>
       <c r="P66" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="Q66" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="R66" t="s">
-        <v>31</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B67" t="s">
-        <v>19</v>
+        <v>199</v>
       </c>
       <c r="C67" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D67" t="s">
         <v>31</v>
@@ -5337,13 +5355,13 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C68" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D68" t="s">
         <v>31</v>
@@ -5393,13 +5411,13 @@
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C69" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D69" t="s">
         <v>31</v>
@@ -5449,13 +5467,13 @@
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="B70" t="s">
         <v>19</v>
       </c>
       <c r="C70" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="D70" t="s">
         <v>31</v>
@@ -5505,13 +5523,13 @@
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B71" t="s">
         <v>19</v>
       </c>
       <c r="C71" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="D71" t="s">
         <v>31</v>
@@ -5561,13 +5579,13 @@
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B72" t="s">
         <v>19</v>
       </c>
       <c r="C72" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D72" t="s">
         <v>31</v>
@@ -5617,13 +5635,13 @@
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B73" t="s">
         <v>19</v>
       </c>
       <c r="C73" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="D73" t="s">
         <v>31</v>
@@ -5673,13 +5691,13 @@
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B74" t="s">
         <v>19</v>
       </c>
       <c r="C74" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="D74" t="s">
         <v>31</v>
@@ -5729,13 +5747,13 @@
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B75" t="s">
         <v>19</v>
       </c>
       <c r="C75" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D75" t="s">
         <v>31</v>
@@ -5785,13 +5803,13 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B76" t="s">
         <v>19</v>
       </c>
       <c r="C76" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D76" t="s">
         <v>31</v>
@@ -5841,13 +5859,13 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B77" t="s">
         <v>19</v>
       </c>
       <c r="C77" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D77" t="s">
         <v>31</v>
@@ -5897,13 +5915,13 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B78" t="s">
-        <v>224</v>
+        <v>19</v>
       </c>
       <c r="C78" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D78" t="s">
         <v>31</v>
@@ -5953,13 +5971,13 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B79" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C79" t="s">
-        <v>64</v>
+        <v>218</v>
       </c>
       <c r="D79" t="s">
         <v>31</v>
@@ -6009,13 +6027,13 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B80" t="s">
         <v>19</v>
       </c>
       <c r="C80" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D80" t="s">
         <v>31</v>
@@ -6065,13 +6083,13 @@
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B81" t="s">
         <v>19</v>
       </c>
       <c r="C81" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="D81" t="s">
         <v>31</v>
@@ -6121,13 +6139,13 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B82" t="s">
         <v>19</v>
       </c>
       <c r="C82" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D82" t="s">
         <v>31</v>
@@ -6177,13 +6195,13 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B83" t="s">
         <v>19</v>
       </c>
       <c r="C83" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D83" t="s">
         <v>31</v>
@@ -6233,13 +6251,13 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B84" t="s">
-        <v>48</v>
+        <v>228</v>
       </c>
       <c r="C84" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="D84" t="s">
         <v>31</v>
@@ -6289,13 +6307,13 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="B85" t="s">
         <v>48</v>
       </c>
       <c r="C85" t="s">
-        <v>238</v>
+        <v>64</v>
       </c>
       <c r="D85" t="s">
         <v>31</v>
@@ -6345,13 +6363,13 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B86" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C86" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D86" t="s">
         <v>31</v>
@@ -6401,13 +6419,13 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B87" t="s">
         <v>19</v>
       </c>
       <c r="C87" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="D87" t="s">
         <v>31</v>
@@ -6457,13 +6475,13 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B88" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C88" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D88" t="s">
         <v>31</v>
@@ -6513,13 +6531,13 @@
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B89" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C89" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="D89" t="s">
         <v>31</v>
@@ -6569,13 +6587,13 @@
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B90" t="s">
         <v>48</v>
       </c>
       <c r="C90" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D90" t="s">
         <v>31</v>
@@ -6625,13 +6643,13 @@
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B91" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C91" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="D91" t="s">
         <v>31</v>
@@ -6681,13 +6699,13 @@
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B92" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C92" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D92" t="s">
         <v>31</v>
@@ -6737,13 +6755,13 @@
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B93" t="s">
         <v>19</v>
       </c>
       <c r="C93" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D93" t="s">
         <v>31</v>
@@ -6793,13 +6811,13 @@
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B94" t="s">
         <v>48</v>
       </c>
       <c r="C94" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D94" t="s">
         <v>31</v>
@@ -6849,13 +6867,13 @@
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="B95" t="s">
         <v>48</v>
       </c>
       <c r="C95" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="D95" t="s">
         <v>31</v>
@@ -6905,13 +6923,13 @@
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B96" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C96" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D96" t="s">
         <v>31</v>
@@ -6961,13 +6979,13 @@
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="B97" t="s">
         <v>19</v>
       </c>
       <c r="C97" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="D97" t="s">
         <v>31</v>
@@ -7017,13 +7035,13 @@
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B98" t="s">
         <v>19</v>
       </c>
       <c r="C98" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="D98" t="s">
         <v>31</v>
@@ -7073,13 +7091,13 @@
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B99" t="s">
         <v>19</v>
       </c>
       <c r="C99" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="D99" t="s">
         <v>31</v>
@@ -7129,13 +7147,13 @@
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B100" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C100" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="D100" t="s">
         <v>31</v>
@@ -7185,13 +7203,13 @@
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B101" t="s">
-        <v>141</v>
+        <v>48</v>
       </c>
       <c r="C101" t="s">
-        <v>140</v>
+        <v>262</v>
       </c>
       <c r="D101" t="s">
         <v>31</v>
@@ -7241,13 +7259,13 @@
     </row>
     <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="B102" t="s">
-        <v>271</v>
+        <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D102" t="s">
         <v>31</v>
@@ -7297,13 +7315,13 @@
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="B103" t="s">
         <v>19</v>
       </c>
       <c r="C103" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="D103" t="s">
         <v>31</v>
@@ -7353,13 +7371,13 @@
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B104" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C104" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D104" t="s">
         <v>31</v>
@@ -7409,13 +7427,13 @@
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B105" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C105" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="D105" t="s">
         <v>31</v>
@@ -7465,13 +7483,13 @@
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B106" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C106" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D106" t="s">
         <v>31</v>
@@ -7521,13 +7539,13 @@
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B107" t="s">
-        <v>282</v>
+        <v>141</v>
       </c>
       <c r="C107" t="s">
-        <v>283</v>
+        <v>140</v>
       </c>
       <c r="D107" t="s">
         <v>31</v>
@@ -7577,13 +7595,13 @@
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="B108" t="s">
-        <v>48</v>
+        <v>275</v>
       </c>
       <c r="C108" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="D108" t="s">
         <v>31</v>
@@ -7633,13 +7651,13 @@
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B109" t="s">
         <v>19</v>
       </c>
       <c r="C109" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D109" t="s">
         <v>31</v>
@@ -7689,13 +7707,13 @@
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="B110" t="s">
-        <v>289</v>
+        <v>48</v>
       </c>
       <c r="C110" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D110" t="s">
         <v>31</v>
@@ -7745,13 +7763,13 @@
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="B111" t="s">
-        <v>141</v>
+        <v>48</v>
       </c>
       <c r="C111" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="D111" t="s">
         <v>31</v>
@@ -7801,13 +7819,13 @@
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="B112" t="s">
-        <v>141</v>
+        <v>48</v>
       </c>
       <c r="C112" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D112" t="s">
         <v>31</v>
@@ -7857,13 +7875,13 @@
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="B113" t="s">
-        <v>141</v>
+        <v>286</v>
       </c>
       <c r="C113" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D113" t="s">
         <v>31</v>
@@ -7913,13 +7931,13 @@
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B114" t="s">
-        <v>141</v>
+        <v>48</v>
       </c>
       <c r="C114" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="D114" t="s">
         <v>31</v>
@@ -7969,13 +7987,13 @@
     </row>
     <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B115" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C115" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D115" t="s">
         <v>31</v>
@@ -8025,13 +8043,13 @@
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B116" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C116" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="D116" t="s">
         <v>31</v>
@@ -8081,13 +8099,13 @@
     </row>
     <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B117" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="C117" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D117" t="s">
         <v>31</v>
@@ -8137,13 +8155,13 @@
     </row>
     <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="B118" t="s">
         <v>141</v>
       </c>
       <c r="C118" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="D118" t="s">
         <v>31</v>
@@ -8193,13 +8211,13 @@
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="B119" t="s">
-        <v>48</v>
+        <v>141</v>
       </c>
       <c r="C119" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="D119" t="s">
         <v>31</v>
@@ -8249,13 +8267,13 @@
     </row>
     <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="B120" t="s">
-        <v>19</v>
+        <v>141</v>
       </c>
       <c r="C120" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="D120" t="s">
         <v>31</v>
@@ -8305,13 +8323,13 @@
     </row>
     <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B121" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C121" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="D121" t="s">
         <v>31</v>
@@ -8361,13 +8379,13 @@
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B122" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C122" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="D122" t="s">
         <v>31</v>
@@ -8417,13 +8435,13 @@
     </row>
     <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B123" t="s">
         <v>19</v>
       </c>
       <c r="C123" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="D123" t="s">
         <v>31</v>
@@ -8473,13 +8491,13 @@
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B124" t="s">
-        <v>320</v>
+        <v>141</v>
       </c>
       <c r="C124" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="D124" t="s">
         <v>31</v>
@@ -8529,13 +8547,13 @@
     </row>
     <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="B125" t="s">
-        <v>323</v>
+        <v>48</v>
       </c>
       <c r="C125" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="D125" t="s">
         <v>31</v>
@@ -8585,13 +8603,13 @@
     </row>
     <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="B126" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="C126" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="D126" t="s">
         <v>31</v>
@@ -8641,13 +8659,13 @@
     </row>
     <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="B127" t="s">
-        <v>328</v>
+        <v>19</v>
       </c>
       <c r="C127" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="D127" t="s">
         <v>31</v>
@@ -8697,13 +8715,13 @@
     </row>
     <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="B128" t="s">
-        <v>48</v>
+        <v>319</v>
       </c>
       <c r="C128" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="D128" t="s">
         <v>31</v>
@@ -8753,13 +8771,13 @@
     </row>
     <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="B129" t="s">
         <v>19</v>
       </c>
       <c r="C129" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="D129" t="s">
         <v>31</v>
@@ -8809,13 +8827,13 @@
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="B130" t="s">
-        <v>19</v>
+        <v>324</v>
       </c>
       <c r="C130" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="D130" t="s">
         <v>31</v>
@@ -8865,57 +8883,449 @@
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>326</v>
+      </c>
+      <c r="B131" t="s">
+        <v>327</v>
+      </c>
+      <c r="C131" t="s">
+        <v>328</v>
+      </c>
+      <c r="D131" t="s">
+        <v>31</v>
+      </c>
+      <c r="E131" t="s">
+        <v>31</v>
+      </c>
+      <c r="F131" t="s">
+        <v>31</v>
+      </c>
+      <c r="G131" t="s">
+        <v>31</v>
+      </c>
+      <c r="H131" t="s">
+        <v>31</v>
+      </c>
+      <c r="I131" t="s">
+        <v>31</v>
+      </c>
+      <c r="J131" t="s">
+        <v>31</v>
+      </c>
+      <c r="K131" t="s">
+        <v>31</v>
+      </c>
+      <c r="L131" t="s">
+        <v>31</v>
+      </c>
+      <c r="M131" t="s">
+        <v>31</v>
+      </c>
+      <c r="N131" t="s">
+        <v>31</v>
+      </c>
+      <c r="O131" t="s">
+        <v>31</v>
+      </c>
+      <c r="P131" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q131" t="s">
+        <v>31</v>
+      </c>
+      <c r="R131" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>329</v>
+      </c>
+      <c r="B132" t="s">
+        <v>48</v>
+      </c>
+      <c r="C132" t="s">
+        <v>330</v>
+      </c>
+      <c r="D132" t="s">
+        <v>31</v>
+      </c>
+      <c r="E132" t="s">
+        <v>31</v>
+      </c>
+      <c r="F132" t="s">
+        <v>31</v>
+      </c>
+      <c r="G132" t="s">
+        <v>31</v>
+      </c>
+      <c r="H132" t="s">
+        <v>31</v>
+      </c>
+      <c r="I132" t="s">
+        <v>31</v>
+      </c>
+      <c r="J132" t="s">
+        <v>31</v>
+      </c>
+      <c r="K132" t="s">
+        <v>31</v>
+      </c>
+      <c r="L132" t="s">
+        <v>31</v>
+      </c>
+      <c r="M132" t="s">
+        <v>31</v>
+      </c>
+      <c r="N132" t="s">
+        <v>31</v>
+      </c>
+      <c r="O132" t="s">
+        <v>31</v>
+      </c>
+      <c r="P132" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q132" t="s">
+        <v>31</v>
+      </c>
+      <c r="R132" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>331</v>
+      </c>
+      <c r="B133" t="s">
+        <v>332</v>
+      </c>
+      <c r="C133" t="s">
+        <v>333</v>
+      </c>
+      <c r="D133" t="s">
+        <v>31</v>
+      </c>
+      <c r="E133" t="s">
+        <v>31</v>
+      </c>
+      <c r="F133" t="s">
+        <v>31</v>
+      </c>
+      <c r="G133" t="s">
+        <v>31</v>
+      </c>
+      <c r="H133" t="s">
+        <v>31</v>
+      </c>
+      <c r="I133" t="s">
+        <v>31</v>
+      </c>
+      <c r="J133" t="s">
+        <v>31</v>
+      </c>
+      <c r="K133" t="s">
+        <v>31</v>
+      </c>
+      <c r="L133" t="s">
+        <v>31</v>
+      </c>
+      <c r="M133" t="s">
+        <v>31</v>
+      </c>
+      <c r="N133" t="s">
+        <v>31</v>
+      </c>
+      <c r="O133" t="s">
+        <v>31</v>
+      </c>
+      <c r="P133" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q133" t="s">
+        <v>31</v>
+      </c>
+      <c r="R133" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>334</v>
+      </c>
+      <c r="B134" t="s">
+        <v>48</v>
+      </c>
+      <c r="C134" t="s">
+        <v>335</v>
+      </c>
+      <c r="D134" t="s">
+        <v>31</v>
+      </c>
+      <c r="E134" t="s">
+        <v>31</v>
+      </c>
+      <c r="F134" t="s">
+        <v>31</v>
+      </c>
+      <c r="G134" t="s">
+        <v>31</v>
+      </c>
+      <c r="H134" t="s">
+        <v>31</v>
+      </c>
+      <c r="I134" t="s">
+        <v>31</v>
+      </c>
+      <c r="J134" t="s">
+        <v>31</v>
+      </c>
+      <c r="K134" t="s">
+        <v>31</v>
+      </c>
+      <c r="L134" t="s">
+        <v>31</v>
+      </c>
+      <c r="M134" t="s">
+        <v>31</v>
+      </c>
+      <c r="N134" t="s">
+        <v>31</v>
+      </c>
+      <c r="O134" t="s">
+        <v>31</v>
+      </c>
+      <c r="P134" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q134" t="s">
+        <v>31</v>
+      </c>
+      <c r="R134" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>336</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B135" t="s">
+        <v>19</v>
+      </c>
+      <c r="C135" t="s">
+        <v>337</v>
+      </c>
+      <c r="D135" t="s">
+        <v>31</v>
+      </c>
+      <c r="E135" t="s">
+        <v>31</v>
+      </c>
+      <c r="F135" t="s">
+        <v>31</v>
+      </c>
+      <c r="G135" t="s">
+        <v>31</v>
+      </c>
+      <c r="H135" t="s">
+        <v>31</v>
+      </c>
+      <c r="I135" t="s">
+        <v>31</v>
+      </c>
+      <c r="J135" t="s">
+        <v>31</v>
+      </c>
+      <c r="K135" t="s">
+        <v>31</v>
+      </c>
+      <c r="L135" t="s">
+        <v>31</v>
+      </c>
+      <c r="M135" t="s">
+        <v>31</v>
+      </c>
+      <c r="N135" t="s">
+        <v>31</v>
+      </c>
+      <c r="O135" t="s">
+        <v>31</v>
+      </c>
+      <c r="P135" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q135" t="s">
+        <v>31</v>
+      </c>
+      <c r="R135" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>338</v>
+      </c>
+      <c r="B136" t="s">
+        <v>19</v>
+      </c>
+      <c r="C136" t="s">
+        <v>339</v>
+      </c>
+      <c r="D136" t="s">
+        <v>31</v>
+      </c>
+      <c r="E136" t="s">
+        <v>31</v>
+      </c>
+      <c r="F136" t="s">
+        <v>31</v>
+      </c>
+      <c r="G136" t="s">
+        <v>31</v>
+      </c>
+      <c r="H136" t="s">
+        <v>31</v>
+      </c>
+      <c r="I136" t="s">
+        <v>31</v>
+      </c>
+      <c r="J136" t="s">
+        <v>31</v>
+      </c>
+      <c r="K136" t="s">
+        <v>31</v>
+      </c>
+      <c r="L136" t="s">
+        <v>31</v>
+      </c>
+      <c r="M136" t="s">
+        <v>31</v>
+      </c>
+      <c r="N136" t="s">
+        <v>31</v>
+      </c>
+      <c r="O136" t="s">
+        <v>31</v>
+      </c>
+      <c r="P136" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q136" t="s">
+        <v>31</v>
+      </c>
+      <c r="R136" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>340</v>
+      </c>
+      <c r="B137" t="s">
         <v>48</v>
       </c>
-      <c r="C131" t="s">
-        <v>337</v>
-      </c>
-      <c r="D131" t="s">
-        <v>31</v>
-      </c>
-      <c r="E131" t="s">
-        <v>31</v>
-      </c>
-      <c r="F131" t="s">
-        <v>31</v>
-      </c>
-      <c r="G131" t="s">
-        <v>31</v>
-      </c>
-      <c r="H131" t="s">
-        <v>31</v>
-      </c>
-      <c r="I131" t="s">
-        <v>31</v>
-      </c>
-      <c r="J131" t="s">
-        <v>31</v>
-      </c>
-      <c r="K131" t="s">
-        <v>31</v>
-      </c>
-      <c r="L131" t="s">
-        <v>31</v>
-      </c>
-      <c r="M131" t="s">
-        <v>31</v>
-      </c>
-      <c r="N131" t="s">
-        <v>31</v>
-      </c>
-      <c r="O131" t="s">
-        <v>31</v>
-      </c>
-      <c r="P131" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q131" t="s">
-        <v>31</v>
-      </c>
-      <c r="R131" t="s">
+      <c r="C137" t="s">
+        <v>341</v>
+      </c>
+      <c r="D137" t="s">
+        <v>31</v>
+      </c>
+      <c r="E137" t="s">
+        <v>31</v>
+      </c>
+      <c r="F137" t="s">
+        <v>31</v>
+      </c>
+      <c r="G137" t="s">
+        <v>31</v>
+      </c>
+      <c r="H137" t="s">
+        <v>31</v>
+      </c>
+      <c r="I137" t="s">
+        <v>31</v>
+      </c>
+      <c r="J137" t="s">
+        <v>31</v>
+      </c>
+      <c r="K137" t="s">
+        <v>31</v>
+      </c>
+      <c r="L137" t="s">
+        <v>31</v>
+      </c>
+      <c r="M137" t="s">
+        <v>31</v>
+      </c>
+      <c r="N137" t="s">
+        <v>31</v>
+      </c>
+      <c r="O137" t="s">
+        <v>31</v>
+      </c>
+      <c r="P137" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q137" t="s">
+        <v>31</v>
+      </c>
+      <c r="R137" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>342</v>
+      </c>
+      <c r="B138" t="s">
+        <v>332</v>
+      </c>
+      <c r="C138" t="s">
+        <v>343</v>
+      </c>
+      <c r="D138" t="s">
+        <v>31</v>
+      </c>
+      <c r="E138" t="s">
+        <v>31</v>
+      </c>
+      <c r="F138" t="s">
+        <v>31</v>
+      </c>
+      <c r="G138" t="s">
+        <v>31</v>
+      </c>
+      <c r="H138" t="s">
+        <v>31</v>
+      </c>
+      <c r="I138" t="s">
+        <v>31</v>
+      </c>
+      <c r="J138" t="s">
+        <v>31</v>
+      </c>
+      <c r="K138" t="s">
+        <v>31</v>
+      </c>
+      <c r="L138" t="s">
+        <v>31</v>
+      </c>
+      <c r="M138" t="s">
+        <v>31</v>
+      </c>
+      <c r="N138" t="s">
+        <v>31</v>
+      </c>
+      <c r="O138" t="s">
+        <v>31</v>
+      </c>
+      <c r="P138" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q138" t="s">
+        <v>31</v>
+      </c>
+      <c r="R138" t="s">
         <v>31</v>
       </c>
     </row>
@@ -8936,28 +9346,28 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="B3" s="1">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="B4" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B5" s="1">
         <v>26</v>
@@ -8965,71 +9375,71 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>160</v>
@@ -9037,79 +9447,79 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>371</v>
+        <v>377</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>160</v>
@@ -9117,111 +9527,111 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>180</v>
@@ -9229,10 +9639,10 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>